<commit_message>
Dataset Final Formato pandas
</commit_message>
<xml_diff>
--- a/Dataset_IMU.xlsx
+++ b/Dataset_IMU.xlsx
@@ -1911,10 +1911,10 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.0211188</v>
+        <v>7.58666666666667e-05</v>
       </c>
       <c r="C106" t="n">
-        <v>0.0211196</v>
+        <v>1.77333333333333e-05</v>
       </c>
       <c r="D106" t="n">
         <v>0</v>
@@ -1925,10 +1925,10 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.0213333333333333</v>
+        <v>-0.000185733333333333</v>
       </c>
       <c r="C107" t="n">
-        <v>0.000213333333333333</v>
+        <v>1.76e-05</v>
       </c>
       <c r="D107" t="n">
         <v>0</v>
@@ -1939,10 +1939,10 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.000213333333333333</v>
+        <v>1.97333333333333e-05</v>
       </c>
       <c r="C108" t="n">
-        <v>0.02112</v>
+        <v>1.34666666666667e-05</v>
       </c>
       <c r="D108" t="n">
         <v>0</v>
@@ -1953,10 +1953,10 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>-0.02112</v>
+        <v>2.41333333333333e-05</v>
       </c>
       <c r="C109" t="n">
-        <v>0.000213333333333333</v>
+        <v>3.45333333333333e-05</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
@@ -1967,10 +1967,10 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>-0.000213333333333333</v>
+        <v>2.32e-05</v>
       </c>
       <c r="C110" t="n">
-        <v>-0.02112</v>
+        <v>4.94666666666667e-05</v>
       </c>
       <c r="D110" t="n">
         <v>0</v>
@@ -1981,10 +1981,10 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>-0.02112</v>
+        <v>3.50666666666667e-05</v>
       </c>
       <c r="C111" t="n">
-        <v>-0.0213333333333333</v>
+        <v>3.41333333333333e-05</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
@@ -1995,10 +1995,10 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.0209066666666667</v>
+        <v>-2.38666666666667e-05</v>
       </c>
       <c r="C112" t="n">
-        <v>0.0209066666666667</v>
+        <v>1.44e-05</v>
       </c>
       <c r="D112" t="n">
         <v>0</v>
@@ -2009,10 +2009,10 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.0213333333333333</v>
+        <v>2.45333333333333e-05</v>
       </c>
       <c r="C113" t="n">
-        <v>0.000213333333333333</v>
+        <v>3.6e-05</v>
       </c>
       <c r="D113" t="n">
         <v>0</v>
@@ -2023,10 +2023,10 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.000213333333333333</v>
+        <v>9.98666666666667e-05</v>
       </c>
       <c r="C114" t="n">
-        <v>0.02112</v>
+        <v>5.37333333333333e-05</v>
       </c>
       <c r="D114" t="n">
         <v>0</v>
@@ -2037,10 +2037,10 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>-0.02112</v>
+        <v>-5.22224046413851e-23</v>
       </c>
       <c r="C115" t="n">
-        <v>0.000213333333333333</v>
+        <v>2.4e-05</v>
       </c>
       <c r="D115" t="n">
         <v>0</v>
@@ -2051,10 +2051,10 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>-0.000213333333333333</v>
+        <v>2.66666666666667e-07</v>
       </c>
       <c r="C116" t="n">
-        <v>-0.02112</v>
+        <v>2.32e-05</v>
       </c>
       <c r="D116" t="n">
         <v>0</v>
@@ -2065,10 +2065,10 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>-0.02112</v>
+        <v>7.2e-06</v>
       </c>
       <c r="C117" t="n">
-        <v>-0.0213333333333333</v>
+        <v>3.78666666666667e-05</v>
       </c>
       <c r="D117" t="n">
         <v>0</v>
@@ -2079,10 +2079,10 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.0209066666666667</v>
+        <v>1.81333333333333e-05</v>
       </c>
       <c r="C118" t="n">
-        <v>0.0209066666666667</v>
+        <v>3.96e-05</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
@@ -2093,10 +2093,10 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.0213333333333333</v>
+        <v>-6.28e-05</v>
       </c>
       <c r="C119" t="n">
-        <v>0.000213333333333333</v>
+        <v>3.06666666666667e-06</v>
       </c>
       <c r="D119" t="n">
         <v>0</v>
@@ -2107,10 +2107,10 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.000213333333333333</v>
+        <v>-0.000111866666666667</v>
       </c>
       <c r="C120" t="n">
-        <v>0.02112</v>
+        <v>1.56e-05</v>
       </c>
       <c r="D120" t="n">
         <v>0</v>
@@ -2121,10 +2121,10 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>-0.02112</v>
+        <v>-2.53333333333333e-06</v>
       </c>
       <c r="C121" t="n">
-        <v>0.000213333333333333</v>
+        <v>3.29333333333333e-05</v>
       </c>
       <c r="D121" t="n">
         <v>0</v>
@@ -2135,10 +2135,10 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>-0.000213333333333333</v>
+        <v>-1.65333333333333e-05</v>
       </c>
       <c r="C122" t="n">
-        <v>-0.02112</v>
+        <v>3.38666666666667e-05</v>
       </c>
       <c r="D122" t="n">
         <v>0</v>
@@ -2149,10 +2149,10 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>-0.02112</v>
+        <v>-7.6e-06</v>
       </c>
       <c r="C123" t="n">
-        <v>-0.0213333333333333</v>
+        <v>1.17333333333333e-05</v>
       </c>
       <c r="D123" t="n">
         <v>0</v>
@@ -2163,10 +2163,10 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.0209066666666667</v>
+        <v>8e-06</v>
       </c>
       <c r="C124" t="n">
-        <v>0.0209066666666667</v>
+        <v>3.14666666666667e-05</v>
       </c>
       <c r="D124" t="n">
         <v>0</v>
@@ -2177,10 +2177,10 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.0213333333333333</v>
+        <v>-4.33333333333333e-05</v>
       </c>
       <c r="C125" t="n">
-        <v>0.000213333333333333</v>
+        <v>-3.46666666666667e-06</v>
       </c>
       <c r="D125" t="n">
         <v>0</v>
@@ -2191,10 +2191,10 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.000213333333333333</v>
+        <v>1.49333333333333e-05</v>
       </c>
       <c r="C126" t="n">
-        <v>0.02112</v>
+        <v>1.96e-05</v>
       </c>
       <c r="D126" t="n">
         <v>0</v>
@@ -2205,10 +2205,10 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>-0.02112</v>
+        <v>-3.33333333333333e-05</v>
       </c>
       <c r="C127" t="n">
-        <v>0.000213333333333333</v>
+        <v>1.84e-05</v>
       </c>
       <c r="D127" t="n">
         <v>0</v>
@@ -2219,10 +2219,10 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>-0.000213333333333333</v>
+        <v>-4.29333333333333e-05</v>
       </c>
       <c r="C128" t="n">
-        <v>-0.02112</v>
+        <v>2.21333333333333e-05</v>
       </c>
       <c r="D128" t="n">
         <v>0</v>
@@ -2233,10 +2233,10 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>-0.02112</v>
+        <v>-2.90666666666667e-05</v>
       </c>
       <c r="C129" t="n">
-        <v>-0.0213333333333333</v>
+        <v>2.22666666666667e-05</v>
       </c>
       <c r="D129" t="n">
         <v>0</v>
@@ -2247,10 +2247,10 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>-0.0213333333333333</v>
+        <v>-2.37333333333333e-05</v>
       </c>
       <c r="C130" t="n">
-        <v>-0.0107733333333333</v>
+        <v>1.28e-05</v>
       </c>
       <c r="D130" t="n">
         <v>0</v>
@@ -2261,10 +2261,10 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>-0.0213333333333333</v>
+        <v>-5.69333333333333e-05</v>
       </c>
       <c r="C131" t="n">
-        <v>-0.0106666666666667</v>
+        <v>-1.33333333333333e-05</v>
       </c>
       <c r="D131" t="n">
         <v>0</v>
@@ -2275,10 +2275,10 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>-0.0213333333333333</v>
+        <v>-0.000214933333333333</v>
       </c>
       <c r="C132" t="n">
-        <v>0.00618666666666667</v>
+        <v>-3.14666666666667e-05</v>
       </c>
       <c r="D132" t="n">
         <v>0</v>
@@ -2289,10 +2289,10 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>-0.0213333333333333</v>
+        <v>8.133333333333331e-06</v>
       </c>
       <c r="C133" t="n">
-        <v>0.0106666666666667</v>
+        <v>9.2e-06</v>
       </c>
       <c r="D133" t="n">
         <v>0</v>
@@ -2303,10 +2303,10 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.00394666666666667</v>
+        <v>-3.22666666666667e-05</v>
       </c>
       <c r="C134" t="n">
-        <v>0.0190933333333333</v>
+        <v>4.8e-06</v>
       </c>
       <c r="D134" t="n">
         <v>0</v>
@@ -2317,10 +2317,10 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.0106666666666667</v>
+        <v>-2.44e-05</v>
       </c>
       <c r="C135" t="n">
-        <v>0.0213333333333333</v>
+        <v>1.33333333333333e-07</v>
       </c>
       <c r="D135" t="n">
         <v>0</v>
@@ -2331,10 +2331,10 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0.0106666666666667</v>
+        <v>-9.8e-05</v>
       </c>
       <c r="C136" t="n">
-        <v>0.0129066666666667</v>
+        <v>-2e-05</v>
       </c>
       <c r="D136" t="n">
         <v>0</v>
@@ -2345,10 +2345,10 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.0106666666666667</v>
+        <v>-1.90666666666667e-05</v>
       </c>
       <c r="C137" t="n">
-        <v>0.0106666666666667</v>
+        <v>1.58666666666667e-05</v>
       </c>
       <c r="D137" t="n">
         <v>0</v>
@@ -2359,10 +2359,10 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.0106666666666667</v>
+        <v>3.29333333333333e-05</v>
       </c>
       <c r="C138" t="n">
-        <v>-0.00405333333333333</v>
+        <v>1.21333333333333e-05</v>
       </c>
       <c r="D138" t="n">
         <v>0</v>
@@ -2373,10 +2373,10 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.0106666666666667</v>
+        <v>1.06666666666667e-05</v>
       </c>
       <c r="C139" t="n">
-        <v>-0.0106666666666667</v>
+        <v>-2e-06</v>
       </c>
       <c r="D139" t="n">
         <v>0</v>
@@ -2387,10 +2387,10 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.0106666666666667</v>
+        <v>-1.45333333333333e-05</v>
       </c>
       <c r="C140" t="n">
-        <v>-0.0180266666666667</v>
+        <v>-1.2e-05</v>
       </c>
       <c r="D140" t="n">
         <v>0</v>
@@ -2401,10 +2401,10 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.0106666666666667</v>
+        <v>-6.719999999999999e-05</v>
       </c>
       <c r="C141" t="n">
-        <v>-0.0213333333333333</v>
+        <v>-2.54666666666667e-05</v>
       </c>
       <c r="D141" t="n">
         <v>0</v>
@@ -2415,10 +2415,10 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.00544</v>
+        <v>-2.05333333333333e-05</v>
       </c>
       <c r="C142" t="n">
-        <v>-0.00565333333333333</v>
+        <v>9.46666666666667e-06</v>
       </c>
       <c r="D142" t="n">
         <v>0</v>
@@ -2429,10 +2429,10 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0</v>
+        <v>-8.8e-06</v>
       </c>
       <c r="C143" t="n">
-        <v>0.0106666666666667</v>
+        <v>1.2e-06</v>
       </c>
       <c r="D143" t="n">
         <v>0</v>
@@ -2443,10 +2443,10 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0</v>
+        <v>3.41333333333333e-05</v>
       </c>
       <c r="C144" t="n">
-        <v>0.00234666666666667</v>
+        <v>-5.86666666666667e-06</v>
       </c>
       <c r="D144" t="n">
         <v>0</v>
@@ -2457,10 +2457,10 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0</v>
+        <v>-4.72e-05</v>
       </c>
       <c r="C145" t="n">
-        <v>-0.0106666666666667</v>
+        <v>-3.97333333333333e-05</v>
       </c>
       <c r="D145" t="n">
         <v>0</v>
@@ -2471,10 +2471,10 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.00565333333333333</v>
+        <v>-3.82666666666667e-05</v>
       </c>
       <c r="C146" t="n">
-        <v>0.00629333333333333</v>
+        <v>-1.90666666666667e-05</v>
       </c>
       <c r="D146" t="n">
         <v>0</v>
@@ -2485,10 +2485,10 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.0106666666666667</v>
+        <v>-4.13333333333333e-05</v>
       </c>
       <c r="C147" t="n">
-        <v>0.0112</v>
+        <v>-2.13333333333333e-05</v>
       </c>
       <c r="D147" t="n">
         <v>0</v>
@@ -2499,10 +2499,10 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.0106666666666667</v>
+        <v>-5.24e-05</v>
       </c>
       <c r="C148" t="n">
-        <v>0.0106666666666667</v>
+        <v>-1.58666666666667e-05</v>
       </c>
       <c r="D148" t="n">
         <v>0</v>
@@ -2513,10 +2513,10 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.0106666666666667</v>
+        <v>-0.000118266666666667</v>
       </c>
       <c r="C149" t="n">
-        <v>-0.00746666666666667</v>
+        <v>-9.73333333333333e-06</v>
       </c>
       <c r="D149" t="n">
         <v>0</v>
@@ -2527,10 +2527,10 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.0106666666666667</v>
+        <v>-4.86666666666667e-05</v>
       </c>
       <c r="C150" t="n">
-        <v>-0.0106666666666667</v>
+        <v>-2.73333333333333e-05</v>
       </c>
       <c r="D150" t="n">
         <v>0</v>
@@ -2541,10 +2541,10 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.0106666666666667</v>
+        <v>-2.37333333333333e-05</v>
       </c>
       <c r="C151" t="n">
-        <v>-0.0197333333333333</v>
+        <v>2.05333333333333e-05</v>
       </c>
       <c r="D151" t="n">
         <v>0</v>
@@ -2555,10 +2555,10 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.0106666666666667</v>
+        <v>-1.04e-05</v>
       </c>
       <c r="C152" t="n">
-        <v>-0.0213333333333333</v>
+        <v>8.66666666666667e-06</v>
       </c>
       <c r="D152" t="n">
         <v>0</v>
@@ -2569,10 +2569,10 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.00373333333333333</v>
+        <v>3.37333333333333e-05</v>
       </c>
       <c r="C153" t="n">
-        <v>-0.000533333333333333</v>
+        <v>4.68e-05</v>
       </c>
       <c r="D153" t="n">
         <v>0</v>

</xml_diff>